<commit_message>
cambios en los muestreos de datos
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/Inventarios - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/Inventarios - Muestreo Datos.xlsx
@@ -5,21 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/SpaOnline/ModeloDominio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis ospina\OneDrive\Documentos\GitHub\DOO\SpaOnline\ModeloDominio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{AC151BCF-08BE-47D1-866F-34F469A0DF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C19E8351-DFEF-4B02-84BE-18460CE62AD3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B60DCA-0D04-4033-800E-72C41F795DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
     <sheet name="Objetos de dominio" sheetId="2" r:id="rId2"/>
-    <sheet name="Inventario" sheetId="5" r:id="rId3"/>
-    <sheet name="ProductoInventario" sheetId="3" r:id="rId4"/>
+    <sheet name="ProductoInventario" sheetId="3" r:id="rId3"/>
+    <sheet name="Inventario" sheetId="5" r:id="rId4"/>
+    <sheet name="Sucursal" sheetId="6" r:id="rId5"/>
+    <sheet name="Producto" sheetId="7" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -115,13 +118,100 @@
     <t>Producto Inventario</t>
   </si>
   <si>
-    <t>inventario</t>
-  </si>
-  <si>
     <t>objeto de dominio gestiona el inventario de productos en el spa.</t>
   </si>
   <si>
     <t>Nombre</t>
+  </si>
+  <si>
+    <t>Inventario A</t>
+  </si>
+  <si>
+    <t>Inventarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Producto </t>
+  </si>
+  <si>
+    <t>Objeto de dominio que contiene la informacion de los productos que se van a utilzar en el Spa</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>Correo Electronico</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Combinación única</t>
+  </si>
+  <si>
+    <t>Sucursal Rionegro</t>
+  </si>
+  <si>
+    <t>CL 10 43 A 29</t>
+  </si>
+  <si>
+    <t>SucursalRionegro@gmail.com</t>
+  </si>
+  <si>
+    <t>Sucursal Marinilla</t>
+  </si>
+  <si>
+    <t>CL 63 9 36</t>
+  </si>
+  <si>
+    <t>SucursalMarinilla@gmail.com</t>
+  </si>
+  <si>
+    <t>Sucursal El Poblado</t>
+  </si>
+  <si>
+    <t>CR 2 5 39</t>
+  </si>
+  <si>
+    <t>SucursalPoblado@gmail.com</t>
+  </si>
+  <si>
+    <t>Nombre Sucursal</t>
+  </si>
+  <si>
+    <t>Inventario B</t>
+  </si>
+  <si>
+    <t>Inventario C</t>
+  </si>
+  <si>
+    <t>Sucursal</t>
+  </si>
+  <si>
+    <t>Objeto de dominio que contiene la informacion de la ubicación de las sucursales del Spa</t>
+  </si>
+  <si>
+    <t>Sucursales</t>
+  </si>
+  <si>
+    <t>ProductoporFabricante</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Loción Corporal Hidratante</t>
+  </si>
+  <si>
+    <t>Crema Facial Anti-edad</t>
+  </si>
+  <si>
+    <t>Crema para masajes</t>
   </si>
 </sst>
 </file>
@@ -153,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,8 +262,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -196,12 +292,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -210,9 +319,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -232,8 +338,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -260,20 +396,20 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>115486</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>29002</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>544490</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>86109</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1D0B06C-D250-7983-E2FD-7CF91B90E18B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68F8F916-4033-1E09-68B2-D35D87195798}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -289,8 +425,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="19050"/>
-          <a:ext cx="8497486" cy="3057952"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="11212490" cy="2753109"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -312,16 +448,49 @@
       <sheetName val="Modelo de Dominio Anemico"/>
       <sheetName val="Objetos de dominio"/>
       <sheetName val="Fabricante"/>
-      <sheetName val="Producto"/>
       <sheetName val="ProductoporFabricante"/>
       <sheetName val="Categoria"/>
-      <sheetName val="ProductoInventario"/>
+      <sheetName val="Producto"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3">
+        <row r="2">
+          <cell r="D2" t="str">
+            <v>L'Oréal Paris Revitalift Crema de Día Anti-edad</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="D3" t="str">
+            <v>Dermalogica Daily Microfoliant</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="D4" t="str">
+            <v>Lubriderm Daily Moisture Lotion</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>Cuidado corporal</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>Cuidado facial</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="C4" t="str">
+            <v>Masajes</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
         <row r="2">
           <cell r="E2" t="str">
             <v>Loción Corporal Hidratante-Cuidado corporal</v>
@@ -338,9 +507,48 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Modelo de Dominio Anemico"/>
+      <sheetName val="Objetos de dominio"/>
+      <sheetName val="Pais"/>
+      <sheetName val="Departamento"/>
+      <sheetName val="Ciudad"/>
+      <sheetName val="Sucursal"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="2">
+          <cell r="E2" t="str">
+            <v>Rionegro-Antioquia-Colombia</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="E3" t="str">
+            <v>Marinilla-Antioquia-Colombia</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4" t="str">
+            <v>Medellin-Antioquia-Colombia</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -682,12 +890,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="7"/>
+    <col min="1" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -700,125 +908,110 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="C1:D3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68" style="9" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="9"/>
+    <col min="1" max="1" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>17</v>
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" location="ProductoInventario!A1" display="Producto Inventario" xr:uid="{B6196C86-5494-41DF-B9BA-21C812FFCEC4}"/>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{F8E25110-D015-427A-BE9B-07EAE75C98E4}"/>
+    <hyperlink ref="A2" location="Inventario!A1" display="Inventario" xr:uid="{08D4207E-906D-44A3-91BA-8264295C65C9}"/>
+    <hyperlink ref="A4" location="Producto!A1" display="Producto " xr:uid="{D12D8784-C5F1-4C9E-924B-5D9B902650C1}"/>
+    <hyperlink ref="A5" location="Sucursal!A1" display="Sucursal" xr:uid="{4F7F1C36-0AB8-43C5-9646-DE74A8E02BAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <f>B2&amp;"-"&amp;A2</f>
-        <v>Inventario-1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27757F1-FD83-4C60-A977-3E4A8F875641}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -861,13 +1054,13 @@
       <c r="C2" s="1">
         <v>10</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>12000</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="11">
         <v>45369</v>
       </c>
-      <c r="F2" s="13" t="str">
+      <c r="F2" s="12" t="str">
         <f>B2&amp;"-"&amp;D2&amp;"-"&amp;E2</f>
         <v>Loción Corporal Hidratante-Cuidado corporal-12000-45369</v>
       </c>
@@ -883,13 +1076,13 @@
       <c r="C3" s="1">
         <v>50</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>20000</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>45346</v>
       </c>
-      <c r="F3" s="13" t="str">
+      <c r="F3" s="12" t="str">
         <f>B3&amp;"-"&amp;D3&amp;"-"&amp;E3</f>
         <v>Crema Facial Anti-edad-Cuidado facial-20000-45346</v>
       </c>
@@ -905,15 +1098,345 @@
       <c r="C4" s="1">
         <v>100</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>14500</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>45262</v>
       </c>
-      <c r="F4" s="13" t="str">
+      <c r="F4" s="12" t="str">
         <f>B4&amp;"-"&amp;D4&amp;"-"&amp;E4</f>
         <v>Crema para masajes-Masajes-14500-45262</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>Sucursal!B2</f>
+        <v>Sucursal Rionegro</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>B2&amp;"-"&amp;C2</f>
+        <v>Inventario A-Sucursal Rionegro</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>Sucursal!B3</f>
+        <v>Sucursal Marinilla</v>
+      </c>
+      <c r="D3" s="4" t="str">
+        <f t="shared" ref="D3:D4" si="0">B3&amp;"-"&amp;C3</f>
+        <v>Inventario B-Sucursal Marinilla</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>Sucursal!B4</f>
+        <v>Sucursal El Poblado</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Inventario C-Sucursal El Poblado</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616AB7BE-59CD-4E2E-A27F-E80B84517586}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="16" t="str">
+        <f>[2]Ciudad!E2</f>
+        <v>Rionegro-Antioquia-Colombia</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1">
+        <v>54323243</v>
+      </c>
+      <c r="G2" s="4" t="str">
+        <f>C2&amp;"-"&amp;D2</f>
+        <v>Rionegro-Antioquia-Colombia-CL 10 43 A 29</v>
+      </c>
+      <c r="H2" s="18" t="str">
+        <f>E2&amp;"-"&amp;F2</f>
+        <v>SucursalRionegro@gmail.com-54323243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="16" t="str">
+        <f>[2]Ciudad!E3</f>
+        <v>Marinilla-Antioquia-Colombia</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3214321</v>
+      </c>
+      <c r="G3" s="4" t="str">
+        <f t="shared" ref="G3:G4" si="0">C3&amp;"-"&amp;D3</f>
+        <v>Marinilla-Antioquia-Colombia-CL 63 9 36</v>
+      </c>
+      <c r="H3" s="18" t="str">
+        <f>E3&amp;"-"&amp;F3</f>
+        <v>SucursalMarinilla@gmail.com-3214321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="16" t="str">
+        <f>[2]Ciudad!E4</f>
+        <v>Medellin-Antioquia-Colombia</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5632421</v>
+      </c>
+      <c r="G4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Medellin-Antioquia-Colombia-CR 2 5 39</v>
+      </c>
+      <c r="H4" s="18" t="str">
+        <f>E4&amp;"-"&amp;F4</f>
+        <v>SucursalPoblado@gmail.com-5632421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" location="Ciudad!E2" display="Ciudad!E2" xr:uid="{6A859185-482A-4E86-AA49-3E9EEFE51468}"/>
+    <hyperlink ref="C3:C4" location="Ciudad!E2" display="Ciudad!E2" xr:uid="{56EF309F-826E-4F44-B180-1F93758CC56D}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{6FF34C34-68B2-4B09-92B3-C65F778D8E89}"/>
+    <hyperlink ref="E3:E4" r:id="rId2" display="SucursalRionegr@gmail.com" xr:uid="{F05DC2DA-717E-4092-9BEE-EC90022B064E}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{5127DA5E-9DFB-4F39-B009-24E369C4A597}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{376E2D9D-2151-4286-8229-0A56CEE9CC3B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2AC53C-B366-43EA-9B67-C36A1BBC718F}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="22">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="24" t="str">
+        <f>[1]ProductoporFabricante!D2</f>
+        <v>L'Oréal Paris Revitalift Crema de Día Anti-edad</v>
+      </c>
+      <c r="D2" s="24" t="str">
+        <f>[1]Categoria!C2</f>
+        <v>Cuidado corporal</v>
+      </c>
+      <c r="E2" s="25" t="str">
+        <f>B2&amp;"-"&amp;D2</f>
+        <v>Loción Corporal Hidratante-Cuidado corporal</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="24" t="str">
+        <f>[1]ProductoporFabricante!D3</f>
+        <v>Dermalogica Daily Microfoliant</v>
+      </c>
+      <c r="D3" s="24" t="str">
+        <f>[1]Categoria!C3</f>
+        <v>Cuidado facial</v>
+      </c>
+      <c r="E3" s="25" t="str">
+        <f t="shared" ref="E3:E4" si="0">B3&amp;"-"&amp;D3</f>
+        <v>Crema Facial Anti-edad-Cuidado facial</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="24" t="str">
+        <f>[1]ProductoporFabricante!D4</f>
+        <v>Lubriderm Daily Moisture Lotion</v>
+      </c>
+      <c r="D4" s="24" t="str">
+        <f>[1]Categoria!C4</f>
+        <v>Masajes</v>
+      </c>
+      <c r="E4" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>Crema para masajes-Masajes</v>
       </c>
     </row>
   </sheetData>

</xml_diff>